<commit_message>
Excel File Date is updated
</commit_message>
<xml_diff>
--- a/ParaBank_Playwright_DotNet/Resources/TestData/ParaBankTestData.xlsx
+++ b/ParaBank_Playwright_DotNet/Resources/TestData/ParaBankTestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai\source\repos\ParaBank_Playwright_DotNet\ParaBank_Playwright_DotNet\Resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{404F188E-E4B8-4023-B399-8298197BC097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF56812-5624-4A74-81B8-60E47B42BD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1440" windowWidth="14400" windowHeight="7270" xr2:uid="{7BBDEE1F-3D2D-4B41-9ACE-BAE180019F3F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7BBDEE1F-3D2D-4B41-9ACE-BAE180019F3F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RegisterData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -22,6 +22,164 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Jamal</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>123 Maple Street</t>
+  </si>
+  <si>
+    <t>456 Oak Avenue</t>
+  </si>
+  <si>
+    <t>789 Pine Road</t>
+  </si>
+  <si>
+    <t>101 Birch Boulevar</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>202 Cedar Lane</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>(303) 555-0198</t>
+  </si>
+  <si>
+    <t>(512) 555-1122</t>
+  </si>
+  <si>
+    <t>(206) 555-3344</t>
+  </si>
+  <si>
+    <t>(305) 555-5566</t>
+  </si>
+  <si>
+    <t>(312) 555-7788</t>
+  </si>
+  <si>
+    <t>123-45-6789</t>
+  </si>
+  <si>
+    <t>987-65-4321</t>
+  </si>
+  <si>
+    <t>321-54-9876</t>
+  </si>
+  <si>
+    <t>654-32-1987</t>
+  </si>
+  <si>
+    <t>789-12-3456</t>
+  </si>
+  <si>
+    <t>Passw0rd!</t>
+  </si>
+  <si>
+    <t>Secure123#</t>
+  </si>
+  <si>
+    <t>Sec123456#</t>
+  </si>
+  <si>
+    <t>Qwerty!99</t>
+  </si>
+  <si>
+    <t>Abc123$</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -35,15 +193,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,12 +215,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +552,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AF1997-48D5-4185-91DD-52C0D2D4E717}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" customWidth="1"/>
+    <col min="11" max="11" width="15.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1">
+        <v>80202</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1">
+        <v>73301</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1">
+        <v>98101</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="1">
+        <v>33101</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1">
+        <v>60601</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>